<commit_message>
adding hardhat_deploy for deploying the contract to testnet or mainnet and README.md
</commit_message>
<xml_diff>
--- a/WorkEstimate.xlsx
+++ b/WorkEstimate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isidrojl\Documents\UM FinTech\Challenges\project_3_UM_FinTech_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3749ABE9-19B5-4509-93BE-59A9BB1B9374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F3F082-B004-4D50-8D32-B23FEC598C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5790" yWindow="2020" windowWidth="32610" windowHeight="19580" xr2:uid="{83D1BAF4-EB37-40F1-90A2-0563FC038E14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Univ. of Miami FinTech Boot Camp</t>
   </si>
@@ -71,9 +71,6 @@
     <t>conservative value.</t>
   </si>
   <si>
-    <t xml:space="preserve">Hours for the implementation to this point: </t>
-  </si>
-  <si>
     <t>Time:</t>
   </si>
   <si>
@@ -126,6 +123,38 @@
   </si>
   <si>
     <t>where you can list, buy, sell, transfer NFTs.</t>
+  </si>
+  <si>
+    <t>Complete Functionality</t>
+  </si>
+  <si>
+    <t>Enhanced Functionality</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hours for the implementation to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>present state</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -304,35 +333,18 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
@@ -341,11 +353,29 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -668,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78E3045-F2D5-40E2-B47B-E98E921F146E}">
-  <dimension ref="B2:O27"/>
+  <dimension ref="B2:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -704,505 +734,547 @@
     </row>
     <row r="3" spans="2:15" ht="23.5" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="6"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" spans="2:15" ht="18.5" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
       <c r="C4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="6"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="5"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="6"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="5"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="18" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="6"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="5"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="6"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="5"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="6"/>
+      <c r="C8" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="5"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9" s="8">
+      <c r="C9" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="6">
         <f>10*8*4</f>
         <v>320</v>
       </c>
-      <c r="O9" s="6"/>
+      <c r="O9" s="5"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="6"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="5"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="22">
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="20">
         <f>+N9*G18</f>
         <v>11538.461538461539</v>
       </c>
-      <c r="O11" s="6"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="6"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="6"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="18"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="5"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="18"/>
+      <c r="D14" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="9">
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="21">
         <v>75000</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="8">
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="6">
+        <f>8*4*5</f>
+        <v>160</v>
+      </c>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="6">
+        <f>8*3*8</f>
+        <v>192</v>
+      </c>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B16" s="4"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="6">
         <f>2*8*3</f>
         <v>48</v>
       </c>
-      <c r="O14" s="6"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="8">
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B17" s="4"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="6">
         <f>4*5*8</f>
         <v>160</v>
       </c>
-      <c r="O15" s="6"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="8">
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B18" s="4"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="21">
+        <f>+G14/52/40</f>
+        <v>36.057692307692307</v>
+      </c>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="6">
         <f>3*4*8</f>
         <v>96</v>
       </c>
-      <c r="O16" s="6"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="8">
-        <v>24</v>
-      </c>
-      <c r="O17" s="6"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="9">
-        <f>+G14/52/40</f>
-        <v>36.057692307692307</v>
-      </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="6"/>
+      <c r="O18" s="5"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N19" s="8">
-        <f>SUM(N14:N18)</f>
-        <v>328</v>
-      </c>
-      <c r="O19" s="6"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="6">
+        <v>24</v>
+      </c>
+      <c r="O19" s="5"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N20" s="9">
-        <f>+N19*G18</f>
-        <v>11826.923076923076</v>
-      </c>
-      <c r="O20" s="6"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="5"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B21" s="4"/>
-      <c r="C21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="14"/>
+      <c r="C21" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="N21" s="6">
+        <f>SUM(N13:N20)</f>
+        <v>680</v>
+      </c>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B22" s="4"/>
-      <c r="C22" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="22">
-        <f>+N20+N11</f>
-        <v>23365.384615384617</v>
-      </c>
-      <c r="O22" s="6"/>
+      <c r="C22" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="N22" s="21">
+        <f>+N21*$G$18</f>
+        <v>24519.23076923077</v>
+      </c>
+      <c r="O22" s="5"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B23" s="4"/>
-      <c r="C23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="6"/>
+      <c r="C23" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="10"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B24" s="4"/>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="20">
+        <f>+N22+N11</f>
+        <v>36057.692307692312</v>
+      </c>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B25" s="4"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B26" s="4"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="10">
-        <v>0.3</v>
-      </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="N24" s="9">
-        <f>+N22*G24</f>
-        <v>7009.6153846153848</v>
-      </c>
-      <c r="O24" s="6"/>
-    </row>
-    <row r="25" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="21"/>
-    </row>
-    <row r="26" spans="2:15" ht="16" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="N26" s="24">
-        <f>+N22+N24</f>
-        <v>30375</v>
-      </c>
-      <c r="O26" s="6"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="N26" s="21">
+        <f>+N24*G24</f>
+        <v>10817.307692307693</v>
+      </c>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="4"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
       <c r="L27" s="12"/>
       <c r="M27" s="13"/>
       <c r="N27" s="12"/>
       <c r="O27" s="14"/>
     </row>
+    <row r="28" spans="2:15" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="4"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="N28" s="23">
+        <f>+N24+N26</f>
+        <v>46875.000000000007</v>
+      </c>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>